<commit_message>
Added the correct youtube link
</commit_message>
<xml_diff>
--- a/MatchTA_Server/Capstone_Input_Files/File2-TA_Grader Avail and Preferences and special request from instrutors - 2025.xlsx
+++ b/MatchTA_Server/Capstone_Input_Files/File2-TA_Grader Avail and Preferences and special request from instrutors - 2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/768b4079c1f233a9/Senior Classes/Working Project/capstone_server/Capstone_Input_Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/768b4079c1f233a9/Senior Classes/Working Project/MatchTA_Server/Capstone_Input_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_61ADFED21B27EF94C7A955EBB6E5FC69374B841C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{028B49C0-F84C-4632-9A9E-7C881170766C}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_61ADFED21B27EF94C7A955EBB6E5FC69374B841C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22F80D2F-EAFC-471B-A85A-E63A46480260}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TAgraderAvail" sheetId="1" r:id="rId1"/>
@@ -2014,18 +2014,18 @@
   </sheetPr>
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A3" sqref="A3:E41"/>
+      <selection pane="topRight" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.5703125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2672,19 +2672,19 @@
   </sheetPr>
   <dimension ref="A1:I991"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:G56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="35" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="164.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="252.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="35.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
   </cols>
@@ -14210,18 +14210,18 @@
   </sheetPr>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="101.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="230.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
changed the order of sorting in the backend
</commit_message>
<xml_diff>
--- a/MatchTA_Server/Capstone_Input_Files/File2-TA_Grader Avail and Preferences and special request from instrutors - 2025.xlsx
+++ b/MatchTA_Server/Capstone_Input_Files/File2-TA_Grader Avail and Preferences and special request from instrutors - 2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/768b4079c1f233a9/Senior Classes/Working Project/MatchTA_Server/Capstone_Input_Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/768b4079c1f233a9/MatchTA/MatchTA_Server/Capstone_Input_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="8" documentId="11_61ADFED21B27EF94C7A955EBB6E5FC69374B841C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22F80D2F-EAFC-471B-A85A-E63A46480260}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TAgraderAvail" sheetId="1" r:id="rId1"/>
@@ -1720,10 +1720,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2672,8 +2668,8 @@
   </sheetPr>
   <dimension ref="A1:I991"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>